<commit_message>
Voltage Divider and ADC Connector
Added note to include voltage divider on accelerometer signals. Flipped
the drawing of the "ADC Connector". Updated Receiver/Input/Output
harnesses.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Wiring Guide.xlsx
+++ b/Design/CAD/mAEWing1 - Wiring Guide.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Projects\PAAW\Technical\mAEWing1\CAD Definition\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" tabRatio="846" activeTab="2"/>
   </bookViews>
@@ -19,12 +14,12 @@
     <sheet name="50 Pin Harness Wiring" sheetId="6" r:id="rId5"/>
     <sheet name="Receiver Input Output" sheetId="10" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="230">
   <si>
     <t>Description</t>
   </si>
@@ -708,6 +703,12 @@
   </si>
   <si>
     <t>Left wing and Aft CB Accels on one ADC, Right wing and Forward CD Accels on one ADC</t>
+  </si>
+  <si>
+    <t>Separate board with 6 voltage dividers using 2x 47 Kohm Resisors for accelerometer signals, keep common pin out</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
 </sst>
 </file>
@@ -3737,7 +3738,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="15074353" y="6856434"/>
+            <a:off x="19319060" y="6866422"/>
             <a:ext cx="605414" cy="583787"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -3782,16 +3783,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1696244</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1446213</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:rowOff>164307</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>584536</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2084723</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>86349</xdr:rowOff>
+      <xdr:rowOff>98255</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3800,7 +3801,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2005807" y="10868026"/>
+          <a:off x="4720432" y="10879932"/>
           <a:ext cx="638510" cy="695948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3844,16 +3845,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>527049</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>253206</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>150019</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1165559</xdr:colOff>
+      <xdr:colOff>284497</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>83967</xdr:rowOff>
+      <xdr:rowOff>95873</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3862,7 +3863,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3801268" y="10865644"/>
+          <a:off x="2920206" y="10877550"/>
           <a:ext cx="638510" cy="695948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3904,7 +3905,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>(Yellw)</a:t>
+            <a:t>(Blue)</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3913,16 +3914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1322387</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>24607</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>159544</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1960897</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>55898</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>93492</xdr:rowOff>
+      <xdr:rowOff>105398</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3931,7 +3932,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4596606" y="10875169"/>
+          <a:off x="2084388" y="10887075"/>
           <a:ext cx="638510" cy="695948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4018,7 +4019,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(Yellw)</a:t>
+            <a:t>(Green)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -4030,16 +4031,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2070099</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>738186</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>169069</xdr:rowOff>
+      <xdr:rowOff>154780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>351172</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1631156</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>103017</xdr:rowOff>
+      <xdr:rowOff>79203</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4048,8 +4049,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5344318" y="10884694"/>
-          <a:ext cx="638510" cy="695948"/>
+          <a:off x="1047749" y="10870405"/>
+          <a:ext cx="892970" cy="686423"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4117,7 +4118,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(Yellw)</a:t>
+            <a:t>(Blu</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> or Grn</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -4129,16 +4154,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>246063</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>154782</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>531813</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>277354</xdr:colOff>
+      <xdr:colOff>1170323</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>88730</xdr:rowOff>
+      <xdr:rowOff>124449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4147,7 +4172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2913063" y="10870407"/>
+          <a:off x="3806032" y="10906126"/>
           <a:ext cx="638510" cy="695948"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10163,7 +10188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -10198,7 +10223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -11573,8 +11598,8 @@
   </sheetPr>
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12872,7 +12897,11 @@
         <v>224</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>228</v>
+      </c>
+    </row>
     <row r="41" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O41" s="26"/>
       <c r="P41" s="79" t="s">
@@ -13963,7 +13992,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14077,7 +14106,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>67</v>
@@ -14137,7 +14166,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>67</v>
@@ -14187,13 +14216,13 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>196</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G8" s="18">
         <v>6</v>
@@ -14375,7 +14404,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>18</v>
+        <v>229</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="16" t="s">
@@ -14388,7 +14417,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6" t="s">
@@ -14414,7 +14443,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6" t="s">

</xml_diff>